<commit_message>
update rab dan schedule upload
</commit_message>
<xml_diff>
--- a/public/referensi/dummy participant.xlsx
+++ b/public/referensi/dummy participant.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA DISK\Projects\application generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA DISK\Projects\application generator\application_letters\public\referensi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65062726-BC42-449D-9FC5-3B4A04A5590F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CD9D45-0AC9-4F1A-ACA7-D557C20FD752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4183" yWindow="2597" windowWidth="18514" windowHeight="11280" xr2:uid="{6CA4C54B-CC02-43B2-9E43-2B376088AE04}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15634" xr2:uid="{6CA4C54B-CC02-43B2-9E43-2B376088AE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>Pilih Narasumber dan Moderator</t>
   </si>
@@ -122,23 +122,227 @@
     <t>Tentukan Rundown Susunan Acara</t>
   </si>
   <si>
-    <t>Tanggal</t>
-  </si>
-  <si>
-    <t>Jam Mulai</t>
-  </si>
-  <si>
-    <t>Jam Selesai</t>
-  </si>
-  <si>
-    <t>Acara/Kegiatan</t>
+    <t>Susun Rencana Anggaran Biaya</t>
+  </si>
+  <si>
+    <t>Sub Uraian</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Satuan</t>
+  </si>
+  <si>
+    <t>Harga Satuan</t>
+  </si>
+  <si>
+    <t>Jumlah</t>
+  </si>
+  <si>
+    <t>MAK</t>
+  </si>
+  <si>
+    <t>5123.BGCG.001.065.GS.525122</t>
+  </si>
+  <si>
+    <t>Belanja Barang</t>
+  </si>
+  <si>
+    <t>Makan Pelaksanaan (170 org x 1 keg)</t>
+  </si>
+  <si>
+    <t>Snack Pelaksanaan (170 org x 1 keg)</t>
+  </si>
+  <si>
+    <t>Belanja Jasa</t>
+  </si>
+  <si>
+    <t>Narasumber Luar K/L (1 Org x 3 JPL x 1 Keg)</t>
+  </si>
+  <si>
+    <t>OJ</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <r>
+      <t>Acara/Kegiatan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Narasumber*</t>
+  </si>
+  <si>
+    <t>Moderator*</t>
+  </si>
+  <si>
+    <r>
+      <t>Kode</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Uraian</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Jam Mulai</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Jam Selesai</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tanggal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>NOTE :</t>
+  </si>
+  <si>
+    <t>17/06/2025</t>
+  </si>
+  <si>
+    <t>Pembukaan</t>
+  </si>
+  <si>
+    <t>Kata Kata Sambutan</t>
+  </si>
+  <si>
+    <t>Materi IoT</t>
+  </si>
+  <si>
+    <t>Bapak Dekan Saintek - Dekan Fakultas Saintek</t>
+  </si>
+  <si>
+    <t>Bapak Pemateri 1 - UIN Yogyakarta; Bapak Pemateri 2 - UIN Malang</t>
+  </si>
+  <si>
+    <t>Ibu Moderator 1 - UIN Yogyakarta</t>
+  </si>
+  <si>
+    <r>
+      <t>Nama</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="170" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="171" formatCode="[$Rp-421]#,##0"/>
+    <numFmt numFmtId="173" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +358,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -163,20 +380,11 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -195,19 +403,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="173" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="[$Rp-421]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="hh:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="hh:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{46AFA3F4-8147-4B9E-A227-C80E47B674F1}"/>
   </tableStyles>
@@ -227,7 +457,7 @@
   <autoFilter ref="A2:D5" xr:uid="{1AD992B8-EE0D-4B3F-97A5-0828F24BF435}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{6C044829-B420-4801-8CA4-DA5709091451}" name="No"/>
-    <tableColumn id="2" xr3:uid="{DC6A4271-0F86-45C4-BA1E-6651B0ABBBB9}" name="Nama"/>
+    <tableColumn id="2" xr3:uid="{DC6A4271-0F86-45C4-BA1E-6651B0ABBBB9}" name="Nama*"/>
     <tableColumn id="3" xr3:uid="{B0829CC5-ADCE-4FA7-A381-782E894794E6}" name="Jabatan-Lembaga"/>
     <tableColumn id="4" xr3:uid="{D5EF2A06-6525-469E-A4A1-39337A158571}" name="Peran"/>
   </tableColumns>
@@ -252,7 +482,7 @@
   <autoFilter ref="L2:N9" xr:uid="{6E4FC7FF-D11D-4BEF-A01C-79B87D1BF661}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BBF37881-D4D5-4C67-A570-AE740C8B0A0D}" name="No"/>
-    <tableColumn id="2" xr3:uid="{820EA3D9-5F45-4698-B7D4-FC09D7909142}" name="Nama"/>
+    <tableColumn id="2" xr3:uid="{820EA3D9-5F45-4698-B7D4-FC09D7909142}" name="Nama*"/>
     <tableColumn id="3" xr3:uid="{9764B332-1AD2-4719-AE69-A3C579B1507F}" name="Jabatan - Lembaga"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -264,12 +494,29 @@
   <autoFilter ref="Q2:W9" xr:uid="{E4C4C60D-F487-4E79-B09D-0CE9C84E8426}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E5727DC7-197F-45D6-90AE-936C75DF8DB9}" name="No"/>
-    <tableColumn id="2" xr3:uid="{0DBAB45F-48CE-49A1-947B-95FE77AC4874}" name="Tanggal"/>
-    <tableColumn id="3" xr3:uid="{A7D7D61F-C307-4E3F-8C5F-9B68EC02F13B}" name="Jam Mulai"/>
-    <tableColumn id="4" xr3:uid="{79E8398A-3B7B-4118-81EB-04500D56AC30}" name="Jam Selesai"/>
-    <tableColumn id="5" xr3:uid="{0BFFE6B4-2A17-4C99-9A9F-5431E8ABB8EF}" name="Acara/Kegiatan"/>
-    <tableColumn id="6" xr3:uid="{658C1FE7-FA21-423D-BE15-CD2ABBA70CE6}" name="Narasumber"/>
-    <tableColumn id="7" xr3:uid="{64B49EE8-7BB2-4E0B-AD0F-296B3C2CCF4E}" name="Moderator"/>
+    <tableColumn id="2" xr3:uid="{0DBAB45F-48CE-49A1-947B-95FE77AC4874}" name="Tanggal**" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{A7D7D61F-C307-4E3F-8C5F-9B68EC02F13B}" name="Jam Mulai**" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{79E8398A-3B7B-4118-81EB-04500D56AC30}" name="Jam Selesai**" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{0BFFE6B4-2A17-4C99-9A9F-5431E8ABB8EF}" name="Acara/Kegiatan*"/>
+    <tableColumn id="6" xr3:uid="{658C1FE7-FA21-423D-BE15-CD2ABBA70CE6}" name="Narasumber*"/>
+    <tableColumn id="7" xr3:uid="{64B49EE8-7BB2-4E0B-AD0F-296B3C2CCF4E}" name="Moderator*"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{765E37C4-EC21-4A19-9B60-D6A75C01F7A7}" name="Table3" displayName="Table3" ref="Z2:AG10" totalsRowShown="0">
+  <autoFilter ref="Z2:AG10" xr:uid="{765E37C4-EC21-4A19-9B60-D6A75C01F7A7}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D12B7DD3-4D10-4D3F-AFA0-02D845B1CA50}" name="No"/>
+    <tableColumn id="2" xr3:uid="{02B0E304-7B47-4C74-88AA-FEFC1C4F7903}" name="Kode*"/>
+    <tableColumn id="3" xr3:uid="{82850E34-84FA-42DD-AE52-DE82CA9F79AC}" name="Uraian*"/>
+    <tableColumn id="4" xr3:uid="{F6D2FB4C-C845-452F-865A-28271B5D961B}" name="Sub Uraian"/>
+    <tableColumn id="5" xr3:uid="{FE731B4F-DB28-490C-B2F9-4F0967AAA8F0}" name="Volume"/>
+    <tableColumn id="6" xr3:uid="{B35ED2FB-5420-4812-A0DD-9EE29C9E88B9}" name="Satuan"/>
+    <tableColumn id="7" xr3:uid="{088546B4-3035-4609-AD28-5713FDFD053A}" name="Harga Satuan" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{562310F5-FC31-4E95-BBE6-F3200F59D8B4}" name="Jumlah" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -592,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59B9331-4B57-4138-BDB9-703DEB8172AA}">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:AG19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -605,54 +852,78 @@
     <col min="3" max="3" width="35.53515625" customWidth="1"/>
     <col min="4" max="4" width="15.07421875" customWidth="1"/>
     <col min="6" max="6" width="7.4609375" customWidth="1"/>
-    <col min="7" max="7" width="18.921875" customWidth="1"/>
+    <col min="7" max="7" width="7.765625" customWidth="1"/>
     <col min="8" max="8" width="23.84375" customWidth="1"/>
-    <col min="9" max="9" width="12.15234375" customWidth="1"/>
+    <col min="9" max="9" width="21.3828125" customWidth="1"/>
     <col min="10" max="10" width="6.61328125" customWidth="1"/>
-    <col min="11" max="11" width="22.61328125" customWidth="1"/>
-    <col min="12" max="12" width="34.61328125" customWidth="1"/>
-    <col min="14" max="14" width="11.07421875" customWidth="1"/>
+    <col min="11" max="11" width="13.07421875" customWidth="1"/>
+    <col min="12" max="12" width="8.3046875" customWidth="1"/>
+    <col min="13" max="13" width="17.4609375" customWidth="1"/>
+    <col min="14" max="14" width="23.4609375" customWidth="1"/>
     <col min="15" max="15" width="20.07421875" customWidth="1"/>
     <col min="16" max="16" width="10.921875" customWidth="1"/>
     <col min="17" max="17" width="9.53515625" customWidth="1"/>
-    <col min="19" max="19" width="21.15234375" customWidth="1"/>
-    <col min="20" max="20" width="24.3046875" customWidth="1"/>
+    <col min="18" max="18" width="16.23046875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="13" style="7" customWidth="1"/>
+    <col min="20" max="20" width="13.3828125" style="7" customWidth="1"/>
+    <col min="21" max="21" width="17.23046875" customWidth="1"/>
+    <col min="22" max="22" width="23.4609375" customWidth="1"/>
+    <col min="23" max="23" width="13.61328125" customWidth="1"/>
+    <col min="26" max="26" width="7" customWidth="1"/>
+    <col min="27" max="27" width="17.921875" customWidth="1"/>
+    <col min="28" max="28" width="28.69140625" customWidth="1"/>
+    <col min="29" max="29" width="37.07421875" customWidth="1"/>
+    <col min="30" max="31" width="10.23046875" customWidth="1"/>
+    <col min="32" max="32" width="10.23046875" style="9" customWidth="1"/>
+    <col min="33" max="33" width="14.84375" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="26.15" x14ac:dyDescent="0.7">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:33" ht="26.15" x14ac:dyDescent="0.7">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="N1" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="Q1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="Z1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -673,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -681,26 +952,50 @@
       <c r="Q2" t="s">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
-        <v>28</v>
+      <c r="R2" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="S2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC2" t="s">
         <v>29</v>
       </c>
-      <c r="T2" t="s">
+      <c r="AD2" t="s">
         <v>30</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AE2" t="s">
         <v>31</v>
       </c>
-      <c r="V2" t="s">
-        <v>7</v>
-      </c>
-      <c r="W2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="AF2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -725,22 +1020,43 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="N3" t="s">
         <v>21</v>
       </c>
+      <c r="O3" t="s">
+        <v>51</v>
+      </c>
       <c r="Q3">
         <v>1</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="R3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" s="7">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="T3" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="U3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -763,7 +1079,7 @@
       <c r="L4">
         <v>2</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="N4" t="s">
@@ -772,11 +1088,51 @@
       <c r="Q4">
         <v>2</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="R4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="T4" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="U4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4">
+        <v>525112</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD4">
+        <v>170</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF4" s="9">
+        <v>30000</v>
+      </c>
+      <c r="AG4" s="10">
+        <f>AD4*AF4</f>
+        <v>5100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
@@ -798,7 +1154,7 @@
       <c r="L5">
         <v>3</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="N5" t="s">
@@ -807,11 +1163,51 @@
       <c r="Q5">
         <v>3</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="R5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="S5" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="T5" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="U5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z5">
+        <v>3</v>
+      </c>
+      <c r="AA5">
+        <v>525112</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD5">
+        <v>170</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" s="9">
+        <v>15000</v>
+      </c>
+      <c r="AG5" s="10">
+        <f>AD5*AF5</f>
+        <v>2550000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.4">
       <c r="G6">
         <v>4</v>
       </c>
@@ -824,16 +1220,41 @@
       <c r="L6">
         <v>4</v>
       </c>
-      <c r="M6" s="2"/>
+      <c r="M6" s="1"/>
       <c r="N6" t="s">
         <v>21</v>
       </c>
       <c r="Q6">
         <v>4</v>
       </c>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="R6" s="5"/>
+      <c r="Z6">
+        <v>4</v>
+      </c>
+      <c r="AA6">
+        <v>525113</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD6">
+        <v>3</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF6" s="9">
+        <v>900000</v>
+      </c>
+      <c r="AG6" s="10">
+        <f>AD6*AF6</f>
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.4">
       <c r="G7">
         <v>5</v>
       </c>
@@ -846,7 +1267,7 @@
       <c r="L7">
         <v>5</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="N7" t="s">
@@ -855,11 +1276,12 @@
       <c r="Q7">
         <v>5</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="R7" s="5"/>
+      <c r="Z7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.4">
       <c r="G8">
         <v>6</v>
       </c>
@@ -872,7 +1294,7 @@
       <c r="L8">
         <v>6</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="N8" t="s">
@@ -881,52 +1303,62 @@
       <c r="Q8">
         <v>6</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="R8" s="5"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.4">
       <c r="L9">
         <v>7</v>
       </c>
-      <c r="M9" s="2"/>
+      <c r="M9" s="1"/>
       <c r="Q9">
         <v>7</v>
       </c>
-      <c r="R9" s="2"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="O16" s="1"/>
+      <c r="R9" s="5"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="O12" s="8"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="O16" s="8"/>
     </row>
     <row r="17" spans="15:15" x14ac:dyDescent="0.4">
-      <c r="O17" s="1"/>
+      <c r="O17" s="8"/>
     </row>
     <row r="18" spans="15:15" x14ac:dyDescent="0.4">
-      <c r="O18" s="1"/>
+      <c r="O18" s="8"/>
     </row>
     <row r="19" spans="15:15" x14ac:dyDescent="0.4">
-      <c r="O19" s="1"/>
+      <c r="O19" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="Z1:AG1"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R1:R1048576" xr:uid="{0AFB3C9C-5ED2-477C-BB53-2FA3CC1D7BBE}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>